<commit_message>
update Excel sample document version to 2.1
</commit_message>
<xml_diff>
--- a/Demo/_Templates/Excel/welcome-200.xlsx
+++ b/Demo/_Templates/Excel/welcome-200.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22425" windowHeight="11970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22423" windowHeight="11974"/>
   </bookViews>
   <sheets>
     <sheet name="New ReoGrid" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
     <t>http://reogrid.net/v1.0/</t>
   </si>
   <si>
-    <t>ReoGrid 2.0</t>
+    <t>ReoGrid 2.1</t>
   </si>
 </sst>
 </file>
@@ -719,9 +719,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="2:13" s="2" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="1.5">
+    <row r="1" spans="2:13" s="2" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="2.6">
       <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
@@ -737,7 +737,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="2:13" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="2:13" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="1.55">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -753,7 +753,7 @@
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
     </row>
-    <row r="11" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="18.45" x14ac:dyDescent="0.5">
       <c r="B11" s="6" t="s">
         <v>1</v>
       </c>
@@ -771,7 +771,7 @@
       </c>
       <c r="L11" s="6"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
@@ -779,7 +779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C15" s="3" t="s">
         <v>18</v>
       </c>
@@ -787,7 +787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
@@ -795,7 +795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
       <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
@@ -803,12 +803,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
       <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.4">
       <c r="C20" s="3" t="s">
         <v>8</v>
       </c>
@@ -816,17 +816,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.4">
       <c r="J21" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.4">
       <c r="C23" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>